<commit_message>
added all cases from excel sheet
</commit_message>
<xml_diff>
--- a/geothermal_surrogate_cases.xlsx
+++ b/geothermal_surrogate_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonchen1974/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colli\OneDrive - JGU\13. Semester\running_geothermalwells.jl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{AF9C8740-A617-5449-9D6E-25D055DB4D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0E59BD-0EE2-4C5E-BA8C-E87CBA448A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{56B75647-DE6C-8F47-9018-5EF867A6E34A}"/>
+    <workbookView xWindow="4044" yWindow="17172" windowWidth="23256" windowHeight="12456" xr2:uid="{56B75647-DE6C-8F47-9018-5EF867A6E34A}"/>
   </bookViews>
   <sheets>
     <sheet name="geothermal_surrogate_cases" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="11">
   <si>
     <t>Case</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>2x2</t>
-  </si>
-  <si>
-    <t>Note: Please simulate for 20 years of operation time and save results at 1, 2, 5, 10, 12, 15, 18 years as well for the transient trajectory</t>
   </si>
 </sst>
 </file>
@@ -557,48 +554,48 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -614,7 +611,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -933,15 +930,15 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="103.33203125" customWidth="1"/>
+    <col min="10" max="10" width="103.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -966,11 +963,9 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -996,7 +991,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1022,7 +1017,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1048,7 +1043,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1074,7 +1069,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1100,7 +1095,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1126,7 +1121,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1152,7 +1147,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1178,7 +1173,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1204,7 +1199,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1230,7 +1225,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1256,7 +1251,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1282,7 +1277,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1308,7 +1303,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1334,7 +1329,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1360,7 +1355,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1386,7 +1381,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1412,7 +1407,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1438,7 +1433,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1464,7 +1459,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1490,7 +1485,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1516,7 +1511,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1542,7 +1537,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1568,7 +1563,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1594,7 +1589,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1620,7 +1615,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1646,7 +1641,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1672,7 +1667,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1698,7 +1693,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1724,7 +1719,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1750,7 +1745,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1776,7 +1771,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>

</xml_diff>